<commit_message>
Added background to read excel sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/data/secTypes.xlsx
+++ b/src/test/resources/data/secTypes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\RestAssuredFramework\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\singh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00703EE-1F42-4D3C-B564-6E3C76C92C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936B042B-DA16-4BE4-B33B-72E9C04A5E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>AAPL</t>
   </si>
@@ -296,7 +296,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added comments to classes
</commit_message>
<xml_diff>
--- a/src/test/resources/data/secTypes.xlsx
+++ b/src/test/resources/data/secTypes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\singh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\singh\Git\JIRARestAssuredFramework\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936B042B-DA16-4BE4-B33B-72E9C04A5E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632368B6-CEF7-481C-9D83-731CBC3511F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>AAPL</t>
   </si>
@@ -296,7 +296,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added delete records function
</commit_message>
<xml_diff>
--- a/src/test/resources/data/secTypes.xlsx
+++ b/src/test/resources/data/secTypes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\singh\Git\JIRARestAssuredFramework\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632368B6-CEF7-481C-9D83-731CBC3511F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC156B20-BDEE-4B2C-A3E6-580D7DBA9842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,11 +16,12 @@
     <sheet name="equity" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>AAPL</t>
   </si>
@@ -296,7 +297,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>